<commit_message>
criado funçoes de somas e preço medio, além da area  do texto para declaração
</commit_message>
<xml_diff>
--- a/PLANILHAS/Testando - Copia.xlsx
+++ b/PLANILHAS/Testando - Copia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25691" windowHeight="13464" activeTab="1"/>
+    <workbookView windowWidth="21108" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -335,18 +335,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.35"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -820,7 +814,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -844,16 +838,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -862,85 +856,85 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -949,34 +943,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1936,10 +1930,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B4:P23"/>
+  <dimension ref="B4:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7777777777778" defaultRowHeight="15.6"/>
@@ -2062,7 +2056,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="11">
-        <f t="shared" si="0"/>
+        <f>F7*D7</f>
         <v>70</v>
       </c>
       <c r="H7" s="7">
@@ -2108,7 +2102,7 @@
         <v>72</v>
       </c>
       <c r="G8" s="11">
-        <f t="shared" ref="G8:G10" si="1">F8*D8</f>
+        <f>F8*D8</f>
         <v>144</v>
       </c>
       <c r="H8" s="7">
@@ -2140,7 +2134,7 @@
         <v>65</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="1"/>
+        <f>F9*D9</f>
         <v>650</v>
       </c>
       <c r="H9" s="7">
@@ -2172,7 +2166,7 @@
         <v>68</v>
       </c>
       <c r="G10" s="11">
-        <f t="shared" si="1"/>
+        <f>F10*D10</f>
         <v>340</v>
       </c>
       <c r="H10" s="7">
@@ -2223,7 +2217,7 @@
         <v>70</v>
       </c>
       <c r="G12" s="11">
-        <f t="shared" ref="G12:G14" si="2">F12*D12</f>
+        <f t="shared" ref="G12:G14" si="1">F12*D12</f>
         <v>210</v>
       </c>
       <c r="H12" s="7">
@@ -2257,7 +2251,7 @@
         <v>85</v>
       </c>
       <c r="G13" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>425</v>
       </c>
       <c r="H13" s="7">
@@ -2290,7 +2284,7 @@
         <v>50</v>
       </c>
       <c r="G14" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H14" s="7">
@@ -2330,7 +2324,7 @@
         <v>70</v>
       </c>
       <c r="G16" s="11">
-        <f t="shared" ref="G16:G19" si="3">F16*D16</f>
+        <f t="shared" ref="G16:G19" si="2">F16*D16</f>
         <v>700</v>
       </c>
       <c r="H16" s="7">
@@ -2361,7 +2355,7 @@
         <v>62</v>
       </c>
       <c r="G17" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>310</v>
       </c>
       <c r="H17" s="7">
@@ -2447,6 +2441,20 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="18"/>
+    </row>
+    <row r="29" spans="6:7">
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="6:7">
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="6:6">
+      <c r="F31" s="20"/>
+    </row>
+    <row r="32" spans="6:6">
+      <c r="F32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>